<commit_message>
components added to pcb
</commit_message>
<xml_diff>
--- a/DOC/Temporizador_V7_SMD.xlsx
+++ b/DOC/Temporizador_V7_SMD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Desktop\GitHub Repos\TemporizadorAC\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B214506-90FA-4E56-BE4C-3B2928DCD9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548320F-8F5C-40CA-9032-7B22EF62DA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6777420-B2DF-4115-B9E1-14C4A8726715}"/>
   </bookViews>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3512E9-E09F-46DD-8BB7-07869849B5BE}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>